<commit_message>
cloudinary unique name file
</commit_message>
<xml_diff>
--- a/trydoc.xlsx
+++ b/trydoc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael-PC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA52B92-DC6B-433F-BF8D-6C340AC9B8D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4188DF66-E0FC-4BC3-8BA6-6FE87260B0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20640" windowHeight="11310" xr2:uid="{E987C773-BE31-4315-B3C6-3EE316AFFFDE}"/>
   </bookViews>
@@ -443,7 +443,7 @@
       <sheetName val="."/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="26">
           <cell r="S26" t="str">
@@ -540,18 +540,18 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -857,7 +857,7 @@
   <dimension ref="A2:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ubicacionService en Solay y Condensadores
</commit_message>
<xml_diff>
--- a/trydoc.xlsx
+++ b/trydoc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\storage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SpringProjects\spring-arquitectura-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17700008-6DFC-462A-8DCF-6633EC36F659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF3DC37-2307-4047-AFDF-26D5AAEE16E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E987C773-BE31-4315-B3C6-3EE316AFFFDE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E987C773-BE31-4315-B3C6-3EE316AFFFDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Form-Envolvente-1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="80">
   <si>
     <t xml:space="preserve">1.1) </t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>Elija una zona</t>
+  </si>
+  <si>
+    <t>Quitar cuando se pruebe UbicacionService</t>
   </si>
 </sst>
 </file>
@@ -835,25 +838,25 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1816,8 +1819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CF74AF-C166-49CD-9383-F6A23EB42D93}">
   <dimension ref="B5:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,25 +1833,28 @@
   <sheetData>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="35">
+      <c r="C6" s="35"/>
+      <c r="D6" s="33">
         <v>7</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="31" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="C7" s="31"/>
+      <c r="C7" s="37"/>
       <c r="D7" s="30" t="s">
         <v>70</v>
       </c>
@@ -2008,8 +2014,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="B5:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,6 +2045,9 @@
       <c r="C7" s="24">
         <v>209</v>
       </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
       <c r="R7" s="19" t="s">
         <v>53</v>
       </c>
@@ -2059,6 +2068,9 @@
       <c r="R10" s="18" t="s">
         <v>50</v>
       </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D15" s="17"/>
     </row>
     <row r="33" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R33" s="17"/>
@@ -2076,15 +2088,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BC8D1A6D9755BA4DACDC023AEE321D58" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="8407c33dbc57c22b02890f9ab05f88f0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0cec9201-ec77-4532-add3-9cf0afa67a3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="414e73d62fa2934c35f1272b2dae311a" ns3:_="">
     <xsd:import namespace="0cec9201-ec77-4532-add3-9cf0afa67a3d"/>
@@ -2230,6 +2233,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2237,14 +2249,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAD8E3A9-B2B1-4B30-AEA3-2BD82C6793AD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB979463-6A6C-4761-86FC-11C8EC0FC4C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2258,6 +2262,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FAD8E3A9-B2B1-4B30-AEA3-2BD82C6793AD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>